<commit_message>
Insert data in specific cell & Reading Data from specific cell
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -52,6 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -588,6 +589,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -599,8 +601,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" t="n">
+        <v>1.0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -625,8 +627,8 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="B2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -651,10 +653,16 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in calender & minor changes in main
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -601,8 +601,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="n">
-        <v>1.0</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restoring to the last known funtional point
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -52,7 +52,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -589,7 +588,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -627,42 +625,15 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="n">
-        <v>1.0</v>
-      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
able to read existing value then update it
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -46,12 +46,16 @@
   </si>
   <si>
     <t>chikne</t>
+  </si>
+  <si>
+    <t>ejas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -588,6 +592,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -625,15 +630,68 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Able to select file and some null pointer error removed
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -631,16 +631,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="14.25">
@@ -648,16 +657,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="4" ht="14.25">
@@ -665,16 +665,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -682,16 +673,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to selectional Present absent panel.
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +50,27 @@
   </si>
   <si>
     <t>ejas</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>yello</t>
+  </si>
+  <si>
+    <t>kanjus</t>
+  </si>
+  <si>
+    <t>maru</t>
+  </si>
+  <si>
+    <t>laila</t>
   </si>
 </sst>
 </file>
@@ -631,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -665,15 +687,71 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="n">
-        <v>6.0</v>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Monthly view panel
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -653,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -679,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="4" ht="14.25">
@@ -687,7 +687,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="5" ht="14.25">

</xml_diff>

<commit_message>
Reading row and creating array out of it
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -614,7 +614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -653,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>4.0</v>
+        <v>11.0</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -687,17 +687,18 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Checkbox added changes in serial attendace marking logic
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>ejas</t>
+  </si>
+  <si>
+    <t>rahul</t>
+  </si>
+  <si>
+    <t>jayesh</t>
   </si>
   <si>
     <t>name</t>
@@ -614,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -653,7 +659,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -679,7 +685,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4" ht="14.25">
@@ -687,7 +693,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -695,10 +701,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25"/>
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="n">
+        <v>37.0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -719,21 +740,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -741,7 +762,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -749,7 +770,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0</v>

</xml_diff>

<commit_message>
View month attendace working
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
   </si>
   <si>
     <t>hansraj</t>
@@ -83,7 +98,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -620,7 +634,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -653,13 +666,28 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="n">
-        <v>4.0</v>
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -679,45 +707,60 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="n">
-        <v>4.0</v>
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4.0</v>
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4.0</v>
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="n">
-        <v>4.0</v>
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="n">
-        <v>37.0</v>
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +773,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -740,21 +782,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -762,7 +804,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -770,7 +812,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>

</xml_diff>

<commit_message>
Selection of which month to mark attendance of selected
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -98,6 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -126,8 +127,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,6 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -687,16 +692,16 @@
         <v>13</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>45</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
       </c>
       <c r="F2">
         <v>8</v>
@@ -728,6 +733,15 @@
         <v>14</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -736,6 +750,15 @@
         <v>15</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
     </row>
@@ -744,6 +767,15 @@
         <v>16</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
@@ -752,6 +784,15 @@
         <v>17</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
     </row>
@@ -760,6 +801,15 @@
         <v>18</v>
       </c>
       <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
@@ -773,6 +823,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>

</xml_diff>

<commit_message>
Help added & changes in looks
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -692,7 +692,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -774,7 +774,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
@@ -856,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -897,7 +897,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
Add function to no button in reset
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -695,7 +695,7 @@
         <v>0.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>
@@ -736,7 +736,7 @@
         <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.0</v>

</xml_diff>